<commit_message>
add code for l1ou
</commit_message>
<xml_diff>
--- a/Data/MainlandAnole_SpeciesList.xlsx
+++ b/Data/MainlandAnole_SpeciesList.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/My Documents/Projects/Mainland Anole Ecomorphs/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/My Documents/Projects/Mainland Anole Ecomorphs/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBFAC2-2635-424E-9119-2AC62BA085F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D9C845-EA34-2D4C-A527-8F2463B104F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3260" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55060" yWindow="2600" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainlandAnole_SpeciesList" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MainlandAnole_SpeciesList!$A$1:$F$201</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="224">
   <si>
     <t>Species</t>
   </si>
@@ -669,6 +672,39 @@
   </si>
   <si>
     <t>smallwoodi</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>Perch Data</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Tw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG </t>
   </si>
 </sst>
 </file>
@@ -1509,15 +1545,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="172" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:XFD200"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1530,8 +1566,14 @@
       <c r="D1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1544,8 +1586,14 @@
       <c r="D2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1558,8 +1606,14 @@
       <c r="D3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1573,7 +1627,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1586,8 +1640,14 @@
       <c r="D5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1600,8 +1660,14 @@
       <c r="D6" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1614,8 +1680,14 @@
       <c r="D7" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1629,7 +1701,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1715,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1656,8 +1728,14 @@
       <c r="D10" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1671,7 +1749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1684,8 +1762,14 @@
       <c r="D12" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1699,7 +1783,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1713,7 +1797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1726,8 +1810,14 @@
       <c r="D15" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1741,7 +1831,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1755,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1768,8 +1858,14 @@
       <c r="D18" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1782,8 +1878,14 @@
       <c r="D19" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>220</v>
+      </c>
+      <c r="F19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1796,8 +1898,14 @@
       <c r="D20" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>219</v>
+      </c>
+      <c r="F20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1811,7 +1919,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1824,8 +1932,14 @@
       <c r="D22" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1853,7 +1967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1867,7 +1981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1881,7 +1995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1895,7 +2009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1909,7 +2023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1923,7 +2037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1937,7 +2051,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1950,8 +2064,14 @@
       <c r="D31" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1965,7 +2085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1979,7 +2099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -1992,8 +2112,14 @@
       <c r="D34" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>221</v>
+      </c>
+      <c r="F34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2007,7 +2133,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -2021,7 +2147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -2034,8 +2160,14 @@
       <c r="D37" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -2048,8 +2180,14 @@
       <c r="D38" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>219</v>
+      </c>
+      <c r="F38" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -2063,7 +2201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -2077,7 +2215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -2090,8 +2228,14 @@
       <c r="D41" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2105,7 +2249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2118,8 +2262,14 @@
       <c r="D43" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>214</v>
+      </c>
+      <c r="F43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -2132,8 +2282,14 @@
       <c r="D44" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>214</v>
+      </c>
+      <c r="F44" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2146,8 +2302,14 @@
       <c r="D45" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>214</v>
+      </c>
+      <c r="F45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -2161,7 +2323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -2175,7 +2337,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -2189,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -2202,8 +2364,14 @@
       <c r="D49" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>220</v>
+      </c>
+      <c r="F49" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -2217,7 +2385,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -2231,7 +2399,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -2244,8 +2412,14 @@
       <c r="D52" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>221</v>
+      </c>
+      <c r="F52" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -2259,7 +2433,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -2273,7 +2447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2287,7 +2461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -2300,8 +2474,14 @@
       <c r="D56" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>220</v>
+      </c>
+      <c r="F56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -2315,7 +2495,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -2329,7 +2509,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -2343,7 +2523,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -2356,8 +2536,14 @@
       <c r="D60" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>217</v>
+      </c>
+      <c r="F60" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -2371,7 +2557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -2385,7 +2571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -2399,7 +2585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -2412,8 +2598,14 @@
       <c r="D64" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>220</v>
+      </c>
+      <c r="F64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -2426,8 +2618,14 @@
       <c r="D65" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>222</v>
+      </c>
+      <c r="F65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -2441,7 +2639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -2454,8 +2652,14 @@
       <c r="D67" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>217</v>
+      </c>
+      <c r="F67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -2469,7 +2673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -2482,8 +2686,14 @@
       <c r="D69" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>214</v>
+      </c>
+      <c r="F69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2496,8 +2706,14 @@
       <c r="D70" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>218</v>
+      </c>
+      <c r="F70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2511,7 +2727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2525,7 +2741,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -2539,7 +2755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -2552,8 +2768,14 @@
       <c r="D74" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>223</v>
+      </c>
+      <c r="F74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -2567,7 +2789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -2580,8 +2802,14 @@
       <c r="D76" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -2594,8 +2822,14 @@
       <c r="D77" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>219</v>
+      </c>
+      <c r="F77" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -2609,7 +2843,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -2622,8 +2856,14 @@
       <c r="D79" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>214</v>
+      </c>
+      <c r="F79" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -2637,7 +2877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -2650,8 +2890,14 @@
       <c r="D81" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>218</v>
+      </c>
+      <c r="F81" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -2665,7 +2911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -2678,8 +2924,14 @@
       <c r="D83" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>218</v>
+      </c>
+      <c r="F83" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -2693,7 +2945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -2707,7 +2959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -2720,8 +2972,14 @@
       <c r="D86" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>216</v>
+      </c>
+      <c r="F86" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -2735,7 +2993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>97</v>
       </c>
@@ -2749,7 +3007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>98</v>
       </c>
@@ -2763,7 +3021,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>99</v>
       </c>
@@ -2777,7 +3035,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -2790,8 +3048,14 @@
       <c r="D91" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="s">
+        <v>219</v>
+      </c>
+      <c r="F91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -2805,7 +3069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -2818,8 +3082,14 @@
       <c r="D93" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" t="s">
+        <v>221</v>
+      </c>
+      <c r="F93" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -2832,8 +3102,14 @@
       <c r="D94" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
+        <v>219</v>
+      </c>
+      <c r="F94" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>104</v>
       </c>
@@ -2846,8 +3122,14 @@
       <c r="D95" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="s">
+        <v>220</v>
+      </c>
+      <c r="F95" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>105</v>
       </c>
@@ -2861,7 +3143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -2875,7 +3157,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -2889,7 +3171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>108</v>
       </c>
@@ -2903,7 +3185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>109</v>
       </c>
@@ -2917,7 +3199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -2930,8 +3212,14 @@
       <c r="D101" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>214</v>
+      </c>
+      <c r="F101" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -2945,7 +3233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -2959,7 +3247,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -2973,7 +3261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -2986,8 +3274,14 @@
       <c r="D105" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>217</v>
+      </c>
+      <c r="F105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -3001,7 +3295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -3015,7 +3309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -3029,7 +3323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -3043,7 +3337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -3056,8 +3350,14 @@
       <c r="D110" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" t="s">
+        <v>214</v>
+      </c>
+      <c r="F110" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -3071,7 +3371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -3085,7 +3385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -3098,8 +3398,14 @@
       <c r="D113" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" t="s">
+        <v>214</v>
+      </c>
+      <c r="F113" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -3113,7 +3419,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -3127,7 +3433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>125</v>
       </c>
@@ -3141,7 +3447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>126</v>
       </c>
@@ -3155,7 +3461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>127</v>
       </c>
@@ -3168,8 +3474,14 @@
       <c r="D118" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118" t="s">
+        <v>220</v>
+      </c>
+      <c r="F118" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>128</v>
       </c>
@@ -3183,7 +3495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>129</v>
       </c>
@@ -3197,7 +3509,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>130</v>
       </c>
@@ -3210,8 +3522,14 @@
       <c r="D121" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121" t="s">
+        <v>218</v>
+      </c>
+      <c r="F121" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>131</v>
       </c>
@@ -3225,7 +3543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>132</v>
       </c>
@@ -3239,7 +3557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>133</v>
       </c>
@@ -3252,8 +3570,14 @@
       <c r="D124" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124" t="s">
+        <v>217</v>
+      </c>
+      <c r="F124" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>134</v>
       </c>
@@ -3266,8 +3590,14 @@
       <c r="D125" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125" t="s">
+        <v>218</v>
+      </c>
+      <c r="F125" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>135</v>
       </c>
@@ -3281,7 +3611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -3295,7 +3625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -3309,7 +3639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -3323,7 +3653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>139</v>
       </c>
@@ -3337,7 +3667,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>140</v>
       </c>
@@ -3351,7 +3681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>141</v>
       </c>
@@ -3365,7 +3695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>142</v>
       </c>
@@ -3379,7 +3709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -3393,7 +3723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>144</v>
       </c>
@@ -3407,7 +3737,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>145</v>
       </c>
@@ -3421,7 +3751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>146</v>
       </c>
@@ -3435,7 +3765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>147</v>
       </c>
@@ -3448,8 +3778,14 @@
       <c r="D138" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138" t="s">
+        <v>219</v>
+      </c>
+      <c r="F138" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>148</v>
       </c>
@@ -3462,8 +3798,14 @@
       <c r="D139" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139" t="s">
+        <v>217</v>
+      </c>
+      <c r="F139" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -3476,8 +3818,14 @@
       <c r="D140" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140" t="s">
+        <v>219</v>
+      </c>
+      <c r="F140" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>150</v>
       </c>
@@ -3490,8 +3838,14 @@
       <c r="D141" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141" t="s">
+        <v>218</v>
+      </c>
+      <c r="F141" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>151</v>
       </c>
@@ -3504,8 +3858,14 @@
       <c r="D142" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142" t="s">
+        <v>219</v>
+      </c>
+      <c r="F142" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>152</v>
       </c>
@@ -3519,7 +3879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>153</v>
       </c>
@@ -3533,7 +3893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>154</v>
       </c>
@@ -3547,7 +3907,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>155</v>
       </c>
@@ -3560,8 +3920,14 @@
       <c r="D146" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E146" t="s">
+        <v>214</v>
+      </c>
+      <c r="F146" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>156</v>
       </c>
@@ -3574,8 +3940,14 @@
       <c r="D147" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147" t="s">
+        <v>218</v>
+      </c>
+      <c r="F147" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>157</v>
       </c>
@@ -3588,8 +3960,14 @@
       <c r="D148" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E148" t="s">
+        <v>220</v>
+      </c>
+      <c r="F148" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>158</v>
       </c>
@@ -3603,7 +3981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>159</v>
       </c>
@@ -3617,7 +3995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>160</v>
       </c>
@@ -3631,7 +4009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>161</v>
       </c>
@@ -3645,7 +4023,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>162</v>
       </c>
@@ -3659,7 +4037,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>163</v>
       </c>
@@ -3673,7 +4051,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>164</v>
       </c>
@@ -3687,7 +4065,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>165</v>
       </c>
@@ -3700,8 +4078,14 @@
       <c r="D156" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E156" t="s">
+        <v>214</v>
+      </c>
+      <c r="F156" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>166</v>
       </c>
@@ -3715,7 +4099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>167</v>
       </c>
@@ -3729,7 +4113,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>168</v>
       </c>
@@ -3742,8 +4126,14 @@
       <c r="D159" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159" t="s">
+        <v>219</v>
+      </c>
+      <c r="F159" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>169</v>
       </c>
@@ -3756,8 +4146,14 @@
       <c r="D160" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E160" t="s">
+        <v>214</v>
+      </c>
+      <c r="F160" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>170</v>
       </c>
@@ -3771,7 +4167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>171</v>
       </c>
@@ -3784,8 +4180,14 @@
       <c r="D162" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E162" t="s">
+        <v>218</v>
+      </c>
+      <c r="F162" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>172</v>
       </c>
@@ -3799,7 +4201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>173</v>
       </c>
@@ -3812,8 +4214,14 @@
       <c r="D164" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E164" t="s">
+        <v>6</v>
+      </c>
+      <c r="F164" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>174</v>
       </c>
@@ -3827,7 +4235,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>175</v>
       </c>
@@ -3841,7 +4249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>176</v>
       </c>
@@ -3855,7 +4263,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>177</v>
       </c>
@@ -3868,8 +4276,14 @@
       <c r="D168" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E168" t="s">
+        <v>217</v>
+      </c>
+      <c r="F168" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>178</v>
       </c>
@@ -3883,7 +4297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>179</v>
       </c>
@@ -3897,7 +4311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>180</v>
       </c>
@@ -3911,7 +4325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>181</v>
       </c>
@@ -3925,7 +4339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>182</v>
       </c>
@@ -3939,7 +4353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>183</v>
       </c>
@@ -3953,7 +4367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>184</v>
       </c>
@@ -3967,7 +4381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>185</v>
       </c>
@@ -3981,7 +4395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>186</v>
       </c>
@@ -3995,7 +4409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>187</v>
       </c>
@@ -4008,8 +4422,14 @@
       <c r="D178" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E178" t="s">
+        <v>6</v>
+      </c>
+      <c r="F178" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>188</v>
       </c>
@@ -4022,8 +4442,14 @@
       <c r="D179" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
+        <v>218</v>
+      </c>
+      <c r="F179" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>189</v>
       </c>
@@ -4037,7 +4463,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>190</v>
       </c>
@@ -4051,7 +4477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>191</v>
       </c>
@@ -4065,7 +4491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>192</v>
       </c>
@@ -4078,8 +4504,14 @@
       <c r="D183" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E183" t="s">
+        <v>219</v>
+      </c>
+      <c r="F183" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>193</v>
       </c>
@@ -4093,7 +4525,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>194</v>
       </c>
@@ -4107,7 +4539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>195</v>
       </c>
@@ -4121,7 +4553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>196</v>
       </c>
@@ -4135,7 +4567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>197</v>
       </c>
@@ -4149,7 +4581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>198</v>
       </c>
@@ -4163,7 +4595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>201</v>
       </c>
@@ -4174,10 +4606,10 @@
         <v>23</v>
       </c>
       <c r="D190" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>202</v>
       </c>
@@ -4188,10 +4620,16 @@
         <v>23</v>
       </c>
       <c r="D191" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="E191" t="s">
+        <v>219</v>
+      </c>
+      <c r="F191" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>203</v>
       </c>
@@ -4204,8 +4642,14 @@
       <c r="D192" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E192" t="s">
+        <v>220</v>
+      </c>
+      <c r="F192" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>204</v>
       </c>
@@ -4219,7 +4663,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>205</v>
       </c>
@@ -4233,7 +4677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>206</v>
       </c>
@@ -4247,7 +4691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>207</v>
       </c>
@@ -4261,7 +4705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>208</v>
       </c>
@@ -4275,7 +4719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -4289,7 +4733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>210</v>
       </c>
@@ -4303,7 +4747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>211</v>
       </c>
@@ -4316,8 +4760,14 @@
       <c r="D200" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E200" t="s">
+        <v>218</v>
+      </c>
+      <c r="F200" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>212</v>
       </c>
@@ -4332,6 +4782,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F201" xr:uid="{3252C1F9-D4C5-6D48-84BF-A0F1B64DF84B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D189">
     <sortCondition ref="A2:A189"/>
   </sortState>

</xml_diff>

<commit_message>
touches on the species
</commit_message>
<xml_diff>
--- a/Data/MainlandAnole_SpeciesList.xlsx
+++ b/Data/MainlandAnole_SpeciesList.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Documents/My Documents/Projects/Mainland Anole Ecomorphs/Code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA748337-D6FC-A447-B6C3-09ED7CB07245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC06ADC5-FDE4-964C-853D-4102CDACE92F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainlandAnole_SpeciesList" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MainlandAnole_SpeciesList!$A$1:$E$204</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MainlandAnole_SpeciesList!$A$1:$E$205</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="227">
   <si>
     <t>Species</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>Island</t>
+  </si>
+  <si>
+    <t>oligaspis</t>
   </si>
 </sst>
 </file>
@@ -1041,13 +1044,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,10 +1215,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1262,7 +1266,24 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1572,13 +1593,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="172" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193"/>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1700,19 +1725,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" s="1"/>
+      <c r="D8" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1941,33 +1966,33 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2052,7 +2077,7 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -2166,19 +2191,19 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2341,16 +2366,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B49" t="s">
-        <v>18</v>
-      </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2400,16 +2425,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B53" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="B53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2448,19 +2473,19 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E56" s="3"/>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -2542,51 +2567,51 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E62" s="3"/>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="D63" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="D64" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2608,16 +2633,16 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="4" t="s">
         <v>199</v>
       </c>
       <c r="E66" t="s">
@@ -2746,16 +2771,16 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="A75" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="4" t="s">
         <v>199</v>
       </c>
       <c r="E75" t="s">
@@ -2873,16 +2898,16 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="A83" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B83" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="B83" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>199</v>
       </c>
       <c r="E83" t="s">
@@ -2924,16 +2949,16 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="A86" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B86" t="s">
-        <v>18</v>
-      </c>
-      <c r="C86" t="s">
-        <v>18</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="B86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3121,19 +3146,19 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E99" s="2" t="s">
+      <c r="D99" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3265,16 +3290,16 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="A108" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B108" t="s">
-        <v>18</v>
-      </c>
-      <c r="C108" t="s">
-        <v>18</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="B108" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3501,19 +3526,19 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E124" s="3"/>
+      <c r="B124" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
@@ -3623,39 +3648,42 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>129</v>
-      </c>
-      <c r="B132" t="s">
-        <v>8</v>
-      </c>
-      <c r="C132" t="s">
-        <v>8</v>
-      </c>
-      <c r="D132" t="s">
-        <v>199</v>
-      </c>
-      <c r="E132" t="s">
-        <v>215</v>
+      <c r="A132" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D133" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E133" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
         <v>18</v>
@@ -3669,55 +3697,55 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D135" t="s">
-        <v>199</v>
-      </c>
-      <c r="E135" t="s">
-        <v>214</v>
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C136" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D136" t="s">
         <v>199</v>
       </c>
       <c r="E136" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B137" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E137" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B138" t="s">
         <v>18</v>
@@ -3731,7 +3759,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B139" t="s">
         <v>18</v>
@@ -3745,52 +3773,52 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>136</v>
+      </c>
+      <c r="B140" t="s">
+        <v>18</v>
+      </c>
+      <c r="C140" t="s">
+        <v>18</v>
+      </c>
+      <c r="D140" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>137</v>
       </c>
-      <c r="B140" t="s">
-        <v>18</v>
-      </c>
-      <c r="C140" t="s">
-        <v>18</v>
-      </c>
-      <c r="D140" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+      <c r="B141" t="s">
+        <v>18</v>
+      </c>
+      <c r="C141" t="s">
+        <v>18</v>
+      </c>
+      <c r="D141" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E141" s="1" t="s">
+      <c r="D142" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>139</v>
-      </c>
-      <c r="B142" t="s">
-        <v>18</v>
-      </c>
-      <c r="C142" t="s">
-        <v>18</v>
-      </c>
-      <c r="D142" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B143" t="s">
         <v>18</v>
@@ -3804,7 +3832,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B144" t="s">
         <v>18</v>
@@ -3818,58 +3846,58 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>141</v>
+      </c>
+      <c r="B145" t="s">
+        <v>18</v>
+      </c>
+      <c r="C145" t="s">
+        <v>18</v>
+      </c>
+      <c r="D145" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>142</v>
       </c>
-      <c r="B145" t="s">
-        <v>18</v>
-      </c>
-      <c r="C145" t="s">
-        <v>18</v>
-      </c>
-      <c r="D145" t="s">
+      <c r="B146" t="s">
+        <v>18</v>
+      </c>
+      <c r="C146" t="s">
+        <v>18</v>
+      </c>
+      <c r="D146" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B147" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E146" s="1" t="s">
+      <c r="D147" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E147" s="1" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>144</v>
-      </c>
-      <c r="B147" t="s">
-        <v>18</v>
-      </c>
-      <c r="C147" t="s">
-        <v>2</v>
-      </c>
-      <c r="D147" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B148" t="s">
         <v>18</v>
       </c>
       <c r="C148" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D148" t="s">
         <v>18</v>
@@ -3877,129 +3905,129 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B149" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C149" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D149" t="s">
-        <v>199</v>
-      </c>
-      <c r="E149" t="s">
-        <v>216</v>
+        <v>18</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="B150" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C150" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D150" t="s">
         <v>199</v>
       </c>
       <c r="E150" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>147</v>
+        <v>210</v>
       </c>
       <c r="B151" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C151" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D151" t="s">
         <v>199</v>
       </c>
       <c r="E151" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B152" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C152" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D152" t="s">
         <v>199</v>
       </c>
       <c r="E152" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B153" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C153" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D153" t="s">
         <v>199</v>
       </c>
       <c r="E153" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B154" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D154" t="s">
         <v>199</v>
       </c>
       <c r="E154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B155" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C155" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D155" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E155" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B156" t="s">
         <v>18</v>
       </c>
       <c r="C156" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D156" t="s">
         <v>18</v>
@@ -4007,13 +4035,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
         <v>18</v>
       </c>
       <c r="C157" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D157" t="s">
         <v>18</v>
@@ -4021,72 +4049,72 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C158" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D158" t="s">
-        <v>199</v>
-      </c>
-      <c r="E158" t="s">
-        <v>216</v>
+        <v>18</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C159" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D159" t="s">
         <v>199</v>
       </c>
       <c r="E159" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C160" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D160" t="s">
         <v>199</v>
       </c>
       <c r="E160" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B161" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D161" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E161" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B162" t="s">
         <v>18</v>
@@ -4095,12 +4123,12 @@
         <v>18</v>
       </c>
       <c r="D162" t="s">
-        <v>225</v>
+        <v>18</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B163" t="s">
         <v>18</v>
@@ -4109,321 +4137,321 @@
         <v>18</v>
       </c>
       <c r="D163" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>159</v>
+      </c>
+      <c r="B164" t="s">
+        <v>18</v>
+      </c>
+      <c r="C164" t="s">
+        <v>18</v>
+      </c>
+      <c r="D164" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>160</v>
       </c>
-      <c r="B164" t="s">
-        <v>18</v>
-      </c>
-      <c r="C164" t="s">
-        <v>18</v>
-      </c>
-      <c r="D164" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
+      <c r="B165" t="s">
+        <v>18</v>
+      </c>
+      <c r="C165" t="s">
+        <v>18</v>
+      </c>
+      <c r="D165" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E165" s="1" t="s">
+      <c r="B166" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E166" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B167" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C167" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D166" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E166" s="2" t="s">
+      <c r="D167" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E167" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="s">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B168" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C168" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D167" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E167" s="2" t="s">
+      <c r="D168" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E168" s="3" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>164</v>
-      </c>
-      <c r="B168" t="s">
-        <v>4</v>
-      </c>
-      <c r="C168" t="s">
-        <v>4</v>
-      </c>
-      <c r="D168" t="s">
-        <v>199</v>
-      </c>
-      <c r="E168" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B169" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D169" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E169" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>165</v>
+      </c>
+      <c r="B170" t="s">
+        <v>18</v>
+      </c>
+      <c r="C170" t="s">
+        <v>18</v>
+      </c>
+      <c r="D170" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B170" t="s">
-        <v>4</v>
-      </c>
-      <c r="C170" t="s">
-        <v>4</v>
-      </c>
-      <c r="D170" t="s">
-        <v>199</v>
-      </c>
-      <c r="E170" t="s">
+      <c r="B171" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E171" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>167</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>23</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C172" t="s">
         <v>23</v>
       </c>
-      <c r="D171" t="s">
-        <v>199</v>
-      </c>
-      <c r="E171" t="s">
+      <c r="D172" t="s">
+        <v>199</v>
+      </c>
+      <c r="E172" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="3" t="s">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B172" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D172" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E172" s="3"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>169</v>
-      </c>
-      <c r="B173" t="s">
-        <v>18</v>
-      </c>
-      <c r="C173" t="s">
-        <v>2</v>
-      </c>
-      <c r="D173" t="s">
-        <v>18</v>
-      </c>
+      <c r="B173" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E173" s="2"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C174" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>199</v>
-      </c>
-      <c r="E174" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B175" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C175" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D175" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E175" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>171</v>
+      </c>
+      <c r="B176" t="s">
+        <v>18</v>
+      </c>
+      <c r="C176" t="s">
+        <v>18</v>
+      </c>
+      <c r="D176" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>172</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" t="s">
         <v>6</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C177" t="s">
         <v>6</v>
       </c>
-      <c r="D176" t="s">
-        <v>199</v>
-      </c>
-      <c r="E176" t="s">
+      <c r="D177" t="s">
+        <v>199</v>
+      </c>
+      <c r="E177" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B179" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="C179" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D178" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E178" s="1" t="s">
+      <c r="D179" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E179" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
         <v>174</v>
       </c>
-      <c r="B179" t="s">
-        <v>18</v>
-      </c>
-      <c r="C179" t="s">
-        <v>18</v>
-      </c>
-      <c r="D179" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
+      <c r="B180" t="s">
+        <v>18</v>
+      </c>
+      <c r="C180" t="s">
+        <v>18</v>
+      </c>
+      <c r="D180" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B180" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E180" s="1" t="s">
+      <c r="B181" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>176</v>
-      </c>
-      <c r="B181" t="s">
-        <v>10</v>
-      </c>
-      <c r="C181" t="s">
-        <v>10</v>
-      </c>
-      <c r="D181" t="s">
-        <v>199</v>
-      </c>
-      <c r="E181" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B182" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C182" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D182" t="s">
-        <v>18</v>
+        <v>199</v>
+      </c>
+      <c r="E182" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B183" t="s">
         <v>18</v>
       </c>
       <c r="C183" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D183" t="s">
         <v>18</v>
@@ -4431,13 +4459,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B184" t="s">
         <v>18</v>
       </c>
       <c r="C184" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D184" t="s">
         <v>18</v>
@@ -4445,7 +4473,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B185" t="s">
         <v>18</v>
@@ -4459,7 +4487,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B186" t="s">
         <v>18</v>
@@ -4473,13 +4501,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B187" t="s">
         <v>18</v>
       </c>
       <c r="C187" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D187" t="s">
         <v>18</v>
@@ -4487,13 +4515,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B188" t="s">
         <v>18</v>
       </c>
       <c r="C188" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D188" t="s">
         <v>18</v>
@@ -4501,13 +4529,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B189" t="s">
         <v>18</v>
       </c>
       <c r="C189" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D189" t="s">
         <v>18</v>
@@ -4515,13 +4543,13 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B190" t="s">
         <v>18</v>
       </c>
       <c r="C190" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D190" t="s">
         <v>18</v>
@@ -4529,109 +4557,109 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C191" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D191" t="s">
-        <v>199</v>
-      </c>
-      <c r="E191" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B192" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C192" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D192" t="s">
         <v>199</v>
       </c>
       <c r="E192" t="s">
-        <v>215</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B193" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D193" t="s">
         <v>199</v>
       </c>
       <c r="E193" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B194" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C194" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D194" t="s">
-        <v>225</v>
+        <v>199</v>
+      </c>
+      <c r="E194" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>188</v>
+      </c>
+      <c r="B195" t="s">
+        <v>18</v>
+      </c>
+      <c r="C195" t="s">
+        <v>18</v>
+      </c>
+      <c r="D195" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B196" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D195" t="s">
-        <v>199</v>
-      </c>
-      <c r="E195" t="s">
+      <c r="D196" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E196" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>189</v>
-      </c>
-      <c r="B196" t="s">
-        <v>18</v>
-      </c>
-      <c r="C196" t="s">
-        <v>18</v>
-      </c>
-      <c r="D196" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B197" t="s">
         <v>18</v>
       </c>
       <c r="C197" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D197" t="s">
         <v>18</v>
@@ -4639,55 +4667,55 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>190</v>
+      </c>
+      <c r="B198" t="s">
+        <v>18</v>
+      </c>
+      <c r="C198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D198" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>191</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B199" t="s">
         <v>23</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C199" t="s">
         <v>23</v>
       </c>
-      <c r="D198" t="s">
-        <v>199</v>
-      </c>
-      <c r="E198" t="s">
+      <c r="D199" t="s">
+        <v>199</v>
+      </c>
+      <c r="E199" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B200" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C200" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D199" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E199" s="1" t="s">
+      <c r="D200" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E200" s="1" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>193</v>
-      </c>
-      <c r="B200" t="s">
-        <v>18</v>
-      </c>
-      <c r="C200" t="s">
-        <v>18</v>
-      </c>
-      <c r="D200" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B201" t="s">
         <v>18</v>
@@ -4701,7 +4729,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B202" t="s">
         <v>18</v>
@@ -4715,7 +4743,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B203" t="s">
         <v>18</v>
@@ -4729,22 +4757,36 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>196</v>
+      </c>
+      <c r="B204" t="s">
+        <v>18</v>
+      </c>
+      <c r="C204" t="s">
+        <v>18</v>
+      </c>
+      <c r="D204" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
         <v>197</v>
       </c>
-      <c r="B204" t="s">
-        <v>18</v>
-      </c>
-      <c r="C204" t="s">
-        <v>18</v>
-      </c>
-      <c r="D204" t="s">
+      <c r="B205" t="s">
+        <v>18</v>
+      </c>
+      <c r="C205" t="s">
+        <v>18</v>
+      </c>
+      <c r="D205" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E204" xr:uid="{3252C1F9-D4C5-6D48-84BF-A0F1B64DF84B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E204">
-      <sortCondition ref="A1:A204"/>
+  <autoFilter ref="A1:E205" xr:uid="{3252C1F9-D4C5-6D48-84BF-A0F1B64DF84B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E205">
+      <sortCondition ref="A1:A205"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D189">

</xml_diff>